<commit_message>
updated files after fixing some bugs
</commit_message>
<xml_diff>
--- a/capstone-backend/drug_template.xlsx
+++ b/capstone-backend/drug_template.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,12 +454,106 @@
           <t>outc_cod</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>dose_amt</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>nda_num</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>route</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>dose_unit</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>dose_form</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>dose_freq</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>dechal</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>rechal</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>role_cod</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
       <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>PS</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>